<commit_message>
No teniamos las validaciones hechas en el servicio
Cambiamos el formato de las celdas del Excel.
</commit_message>
<xml_diff>
--- a/empleados_con_errores_prueba.xlsx
+++ b/empleados_con_errores_prueba.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Iñigo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC623A5-7F1D-4106-9067-7CE9748C0678}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC4BA37-C5C2-4993-A77C-867A7FC78E2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30780" yWindow="2355" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="57">
   <si>
     <t>name</t>
   </si>
@@ -151,9 +151,6 @@
     <t>marta@iem.com</t>
   </si>
   <si>
-    <t>jorge@gmail.com</t>
-  </si>
-  <si>
     <t>elena@iem.com</t>
   </si>
   <si>
@@ -166,36 +163,6 @@
     <t>ruben@iem.com</t>
   </si>
   <si>
-    <t>2024-01-10</t>
-  </si>
-  <si>
-    <t>2023-11-05</t>
-  </si>
-  <si>
-    <t>2024-06-01</t>
-  </si>
-  <si>
-    <t>2022-03-15</t>
-  </si>
-  <si>
-    <t>2023-05-01</t>
-  </si>
-  <si>
-    <t>2022-09-18</t>
-  </si>
-  <si>
-    <t>2023-02-20</t>
-  </si>
-  <si>
-    <t>2024-04-12</t>
-  </si>
-  <si>
-    <t>2023-08-30</t>
-  </si>
-  <si>
-    <t>2022-12-01</t>
-  </si>
-  <si>
     <t>HR001</t>
   </si>
   <si>
@@ -221,13 +188,19 @@
   </si>
   <si>
     <t>NORMAL</t>
+  </si>
+  <si>
+    <t>jorgegtmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,6 +210,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -279,11 +260,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,7 +584,7 @@
     <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
@@ -633,264 +618,267 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="3">
         <v>30</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="5">
+        <v>45301</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H2" t="s">
-        <v>66</v>
+      <c r="H2" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="3">
         <v>28</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="5">
+        <v>45235</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="3">
+        <v>35</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="5">
+        <v>45444</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="3">
+        <v>40</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F5" s="5">
+        <v>44635</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="3">
+        <v>29</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="5">
+        <v>45047</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="3">
+        <v>33</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="5">
+        <v>44822</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="3">
+        <v>31</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="5">
+        <v>44977</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="3">
+        <v>37</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="5">
+        <v>45394</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="3">
+        <v>26</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="5">
+        <v>45168</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G3" t="s">
-        <v>59</v>
-      </c>
-      <c r="H3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4">
-        <v>35</v>
-      </c>
-      <c r="E4" t="s">
-        <v>40</v>
-      </c>
-      <c r="F4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G4" t="s">
-        <v>63</v>
-      </c>
-      <c r="H4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5">
-        <v>40</v>
-      </c>
-      <c r="E5" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6">
-        <v>29</v>
-      </c>
-      <c r="E6" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" t="s">
-        <v>52</v>
-      </c>
-      <c r="G6" t="s">
-        <v>61</v>
-      </c>
-      <c r="H6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7">
-        <v>33</v>
-      </c>
-      <c r="E7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" t="s">
-        <v>62</v>
-      </c>
-      <c r="H7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8">
-        <v>31</v>
-      </c>
-      <c r="E8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="H10" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="3">
+        <v>39</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="5">
+        <v>44896</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="G8" t="s">
-        <v>59</v>
-      </c>
-      <c r="H8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9">
-        <v>37</v>
-      </c>
-      <c r="E9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" t="s">
-        <v>55</v>
-      </c>
-      <c r="G9" t="s">
-        <v>63</v>
-      </c>
-      <c r="H9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D10">
-        <v>26</v>
-      </c>
-      <c r="E10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F10" t="s">
-        <v>56</v>
-      </c>
-      <c r="G10" t="s">
-        <v>60</v>
-      </c>
-      <c r="H10" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" t="s">
-        <v>37</v>
-      </c>
-      <c r="D11">
-        <v>39</v>
-      </c>
-      <c r="E11" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" t="s">
-        <v>57</v>
-      </c>
-      <c r="G11" t="s">
-        <v>58</v>
-      </c>
-      <c r="H11" t="s">
-        <v>65</v>
-      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C12" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Ajustes realizados durante la documentación
</commit_message>
<xml_diff>
--- a/empleados_con_errores_prueba.xlsx
+++ b/empleados_con_errores_prueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC4BA37-C5C2-4993-A77C-867A7FC78E2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6E1BCC-C840-4B18-832C-B47F1A144433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30780" yWindow="2355" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -88,9 +88,6 @@
     <t>Fernández Ruiz</t>
   </si>
   <si>
-    <t>Pérez Gómez</t>
-  </si>
-  <si>
     <t>Sanz Ortega</t>
   </si>
   <si>
@@ -118,9 +115,6 @@
     <t>99887766D</t>
   </si>
   <si>
-    <t>33445566E</t>
-  </si>
-  <si>
     <t>77889900F</t>
   </si>
   <si>
@@ -148,9 +142,6 @@
     <t>luis@iem.com</t>
   </si>
   <si>
-    <t>marta@iem.com</t>
-  </si>
-  <si>
     <t>elena@iem.com</t>
   </si>
   <si>
@@ -191,6 +182,15 @@
   </si>
   <si>
     <t>jorgegtmail.com</t>
+  </si>
+  <si>
+    <t>Alcaide Perez</t>
+  </si>
+  <si>
+    <t>33445566Z</t>
+  </si>
+  <si>
+    <t>martanuevo@iem.com</t>
   </si>
 </sst>
 </file>
@@ -200,7 +200,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,6 +220,14 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -257,10 +265,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -269,8 +278,10 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -576,7 +587,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,22 +636,22 @@
         <v>18</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2" s="3">
         <v>30</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F2" s="5">
         <v>45301</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -651,22 +662,22 @@
         <v>19</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="3">
         <v>28</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F3" s="5">
         <v>45235</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -677,22 +688,22 @@
         <v>20</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4" s="3">
         <v>35</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F4" s="5">
         <v>45444</v>
       </c>
       <c r="G4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -703,22 +714,22 @@
         <v>21</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D5" s="3">
         <v>40</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F5" s="5">
         <v>44635</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -726,25 +737,25 @@
         <v>12</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>22</v>
+        <v>54</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="D6" s="3">
-        <v>29</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>42</v>
+        <v>56</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="F6" s="5">
         <v>45047</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -752,25 +763,25 @@
         <v>13</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D7" s="3">
         <v>33</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F7" s="5">
         <v>44822</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -778,25 +789,25 @@
         <v>14</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D8" s="3">
         <v>31</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F8" s="5">
         <v>44977</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -804,25 +815,25 @@
         <v>15</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D9" s="3">
         <v>37</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F9" s="5">
         <v>45394</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -830,25 +841,25 @@
         <v>16</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D10" s="3">
         <v>26</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F10" s="5">
         <v>45168</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -856,31 +867,34 @@
         <v>17</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D11" s="3">
         <v>39</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F11" s="5">
         <v>44896</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C12" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E6" r:id="rId1" xr:uid="{9289ABAF-A031-44B2-854E-0D59E9EA7491}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>